<commit_message>
Create and check functions to summarize model results
</commit_message>
<xml_diff>
--- a/input/lookup-tables/attributes_model.xlsx
+++ b/input/lookup-tables/attributes_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgangray/Library/CloudStorage/Dropbox/projects/z_archive/ltnc_rxg_2025-01-09/input/lookup-tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgangray/Documents/GitHub/ltnc_rxg/input/lookup-tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD10A8A5-3A54-1D48-B116-938FBBA3B517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1964FA45-B098-8846-A21C-3A2D5F1FA8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="2200" windowWidth="20240" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4360" yWindow="2200" windowWidth="27600" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subset" sheetId="3" r:id="rId1"/>
@@ -25,9 +25,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
   <si>
-    <t>ord</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -145,12 +142,6 @@
     <t>Grazing treatment</t>
   </si>
   <si>
-    <t>lab_subset</t>
-  </si>
-  <si>
-    <t>lab_term</t>
-  </si>
-  <si>
     <t>grazer</t>
   </si>
   <si>
@@ -175,9 +166,6 @@
     <t>New plot</t>
   </si>
   <si>
-    <t>lab_value</t>
-  </si>
-  <si>
     <t>statistic</t>
   </si>
   <si>
@@ -256,10 +244,22 @@
     <t>contrast</t>
   </si>
   <si>
-    <t>lab_contrast</t>
-  </si>
-  <si>
     <t>Ungrazed - Grazed</t>
+  </si>
+  <si>
+    <t>abbr_subset</t>
+  </si>
+  <si>
+    <t>abbr_term</t>
+  </si>
+  <si>
+    <t>abbr_value</t>
+  </si>
+  <si>
+    <t>abbr_contrast</t>
+  </si>
+  <si>
+    <t>order</t>
   </si>
 </sst>
 </file>
@@ -1086,28 +1086,28 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1137,10 +1137,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1148,10 +1148,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1159,10 +1159,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1190,21 +1190,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1234,10 +1234,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1256,10 +1256,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
         <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1267,10 +1267,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1278,10 +1278,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1300,7 +1300,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1313,58 +1313,58 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2019</v>
@@ -1373,15 +1373,15 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>2020</v>
@@ -1390,15 +1390,15 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>2021</v>
@@ -1407,15 +1407,15 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>2022</v>
@@ -1424,248 +1424,248 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
         <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1681,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1694,156 +1694,156 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C3">
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
       </c>
       <c r="C4">
         <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
       </c>
       <c r="C5">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
       </c>
       <c r="C6">
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C7">
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C9">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
       </c>
       <c r="C10">
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create model summary document
</commit_message>
<xml_diff>
--- a/input/lookup-tables/attributes_model.xlsx
+++ b/input/lookup-tables/attributes_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morgangray/Documents/GitHub/ltnc_rxg/input/lookup-tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1964FA45-B098-8846-A21C-3A2D5F1FA8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DE5185-CE91-0042-92FB-BE6380BA5443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="2200" windowWidth="27600" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4360" yWindow="2200" windowWidth="27600" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subset" sheetId="3" r:id="rId1"/>
@@ -18,12 +18,25 @@
     <sheet name="mean" sheetId="4" r:id="rId3"/>
     <sheet name="contrast" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
   <si>
     <t>value</t>
   </si>
@@ -244,9 +257,6 @@
     <t>contrast</t>
   </si>
   <si>
-    <t>Ungrazed - Grazed</t>
-  </si>
-  <si>
     <t>abbr_subset</t>
   </si>
   <si>
@@ -260,6 +270,33 @@
   </si>
   <si>
     <t>order</t>
+  </si>
+  <si>
+    <t>mean(Grazed) - mean(Ungrazed)</t>
+  </si>
+  <si>
+    <t>mean(y5) - mean(y4)</t>
+  </si>
+  <si>
+    <t>mean(y6) - mean(y4)</t>
+  </si>
+  <si>
+    <t>mean(y7) - mean(y4)</t>
+  </si>
+  <si>
+    <t>mean(y6) - mean(y5)</t>
+  </si>
+  <si>
+    <t>mean(y7) - mean(y5)</t>
+  </si>
+  <si>
+    <t>mean(y7) - mean(y6)</t>
+  </si>
+  <si>
+    <t>mean(w) - mean(p)</t>
+  </si>
+  <si>
+    <t>mean(t1) - mean(t0)</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1093,13 +1130,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1190,13 +1227,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1313,16 +1350,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
         <v>47</v>
@@ -1678,32 +1715,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3572E368-099D-C749-B385-CC1B4886C2D0}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1714,7 +1751,7 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
@@ -1722,27 +1759,27 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -1750,13 +1787,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -1764,13 +1801,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C6">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
@@ -1778,13 +1815,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C7">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
@@ -1792,13 +1829,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C8">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
@@ -1806,49 +1843,161 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C11">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
-    <sortCondition ref="C2:C11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D10">
+    <sortCondition ref="C2:C10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>